<commit_message>
added more reandomized dialogue
</commit_message>
<xml_diff>
--- a/Software Development/amicus-bot-framework/resource/food_list.xlsx
+++ b/Software Development/amicus-bot-framework/resource/food_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaewoojang/Desktop/spring2019/cs210b/BMW-2/Software Development/amicus-bot-framework/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD76E166-1FFE-C841-8175-57F8AD9E72B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE96F5E9-FE77-0A42-AF82-B7FFADC5E76F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chains - specific" sheetId="1" r:id="rId1"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2231,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2277,7 +2277,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">

</xml_diff>